<commit_message>
file share in RtcPeerConnection with out multi sunc
</commit_message>
<xml_diff>
--- a/RTCDocuments/RTC이슈및 완료.xlsx
+++ b/RTCDocuments/RTC이슈및 완료.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lee\study\Test-WebRTC\RTCDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FEE3AF-741B-4E3C-8D62-62CEB5194A98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B73F9C5-40F8-4874-BD91-446ED6496582}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>Fire Fox</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,10 +176,6 @@
   </si>
   <si>
     <t>CPU 부하, 조각 녹화파일 Merge 시 실패 우려 ( 테스트 중 )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -894,19 +890,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>x-matroska</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>avc1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>동일  : x-matroska</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>동일 : avc1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Safari : 아이폰 영상 오류 ( 다른건 정상 ), 캔버스 화면 UI 오류, 녹화 불가능 
+모든 PC 브라우저 : 파일업로드 정상 동기화, 캔버스 정상 작동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1296,6 +1289,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1310,33 +1330,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1654,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998AB3B-3CE7-43CD-B034-BC71B811CA97}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1678,10 +1671,10 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="49"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -1706,7 +1699,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>1</v>
@@ -1724,23 +1717,24 @@
         <v>4</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="V3" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="8" t="s">
@@ -1806,22 +1800,22 @@
       <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
+      <c r="I5" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
     </row>
     <row r="6" spans="1:22" ht="17.25" customHeight="1">
       <c r="A6" s="8" t="s">
@@ -1848,22 +1842,22 @@
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="50"/>
-      <c r="U6" s="50"/>
-      <c r="V6" s="50"/>
+      <c r="I6" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="8" t="s">
@@ -1890,13 +1884,13 @@
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
+      <c r="I7" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -1911,7 +1905,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -1931,13 +1925,13 @@
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
+      <c r="I8" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -1972,21 +1966,21 @@
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
+      <c r="I9" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
       <c r="V9" s="12"/>
     </row>
     <row r="10" spans="1:22">
@@ -2004,17 +1998,17 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
+      <c r="I10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
@@ -2025,7 +2019,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>1</v>
@@ -2044,73 +2038,73 @@
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="45" t="s">
-        <v>58</v>
+      <c r="A13" s="54" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="55"/>
+      <c r="B14" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C14" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="36" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="46"/>
-      <c r="B14" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>54</v>
       </c>
       <c r="E14" s="36" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>55</v>
-      </c>
       <c r="C15" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="39" t="s">
         <v>12</v>
@@ -2121,26 +2115,26 @@
       <c r="H15" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="57" t="s">
-        <v>69</v>
+      <c r="I15" s="44" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="47"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>57</v>
-      </c>
       <c r="D16" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>12</v>
@@ -2188,7 +2182,7 @@
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
@@ -2227,26 +2221,26 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A23" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44"/>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="44"/>
+      <c r="A23" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
     </row>
     <row r="24" spans="1:21" ht="18" customHeight="1">
       <c r="A24" s="30"/>
@@ -2270,78 +2264,78 @@
       <c r="S24" s="28"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A25" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
-      <c r="R25" s="48"/>
-      <c r="S25" s="48"/>
-      <c r="T25" s="48"/>
-      <c r="U25" s="48"/>
+      <c r="A25" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
     </row>
     <row r="26" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="48"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="48"/>
-      <c r="U26" s="48"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
     </row>
     <row r="27" spans="1:21" ht="16.5" customHeight="1"/>
     <row r="28" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A28" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="48"/>
-      <c r="U28" s="48"/>
+      <c r="A28" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
     </row>
     <row r="29" spans="1:21" ht="16.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2367,22 +2361,22 @@
       <c r="U29" s="29"/>
     </row>
     <row r="30" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A30" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
+      <c r="A30" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="28"/>
@@ -2392,24 +2386,24 @@
       <c r="U30" s="28"/>
     </row>
     <row r="31" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2419,7 +2413,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -2438,7 +2432,7 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -2457,7 +2451,7 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -2475,7 +2469,13 @@
       <c r="O36" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A23:R23"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:U26"/>
+    <mergeCell ref="A30:N31"/>
+    <mergeCell ref="A28:U28"/>
     <mergeCell ref="I6:V6"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="I8:M8"/>
@@ -2483,12 +2483,7 @@
     <mergeCell ref="I10:Q10"/>
     <mergeCell ref="I9:U9"/>
     <mergeCell ref="I5:V5"/>
-    <mergeCell ref="A23:R23"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:U26"/>
-    <mergeCell ref="A30:N31"/>
-    <mergeCell ref="A28:U28"/>
+    <mergeCell ref="I3:V3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
file upload in server
</commit_message>
<xml_diff>
--- a/RTCDocuments/RTC이슈및 완료.xlsx
+++ b/RTCDocuments/RTC이슈및 완료.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lee\study\Test-WebRTC\RTCDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B73F9C5-40F8-4874-BD91-446ED6496582}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AF2F7-F659-4251-9828-8964C29AE6F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
   </bookViews>
@@ -898,8 +898,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Safari : 아이폰 영상 오류 ( 다른건 정상 ), 캔버스 화면 UI 오류, 녹화 불가능 
-모든 PC 브라우저 : 파일업로드 정상 동기화, 캔버스 정상 작동</t>
+    <t xml:space="preserve">Safari : 아이폰 영상 오류 ( 내영상 자동 재생안됨.. ), 캔버스 화면 UI 오류, 녹화 불가능 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1292,6 +1291,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1314,21 +1328,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1648,7 +1647,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I3" sqref="I3:V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1671,10 +1670,10 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="49"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -1719,22 +1718,22 @@
       <c r="H3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="8" t="s">
@@ -1800,22 +1799,22 @@
       <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="51"/>
+      <c r="V5" s="51"/>
     </row>
     <row r="6" spans="1:22" ht="17.25" customHeight="1">
       <c r="A6" s="8" t="s">
@@ -1842,22 +1841,22 @@
       <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="I6" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="46"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="8" t="s">
@@ -1884,13 +1883,13 @@
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
@@ -1925,13 +1924,13 @@
       <c r="H8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
@@ -1966,21 +1965,21 @@
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
       <c r="V9" s="12"/>
     </row>
     <row r="10" spans="1:22">
@@ -1998,17 +1997,17 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
@@ -2038,7 +2037,7 @@
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="46" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="35" t="s">
@@ -2064,7 +2063,7 @@
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="55"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="35" t="s">
         <v>51</v>
       </c>
@@ -2091,7 +2090,7 @@
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="47" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="38" t="s">
@@ -2120,7 +2119,7 @@
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="56"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="41" t="s">
         <v>55</v>
       </c>
@@ -2221,26 +2220,26 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="53"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
     </row>
     <row r="24" spans="1:21" ht="18" customHeight="1">
       <c r="A24" s="30"/>
@@ -2264,78 +2263,78 @@
       <c r="S24" s="28"/>
     </row>
     <row r="25" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="57"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="49"/>
     </row>
     <row r="26" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="49"/>
     </row>
     <row r="27" spans="1:21" ht="16.5" customHeight="1"/>
     <row r="28" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="49"/>
     </row>
     <row r="29" spans="1:21" ht="16.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2361,22 +2360,22 @@
       <c r="U29" s="29"/>
     </row>
     <row r="30" spans="1:21" ht="20.25" customHeight="1">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="28"/>
@@ -2386,20 +2385,20 @@
       <c r="U30" s="28"/>
     </row>
     <row r="31" spans="1:21" ht="16.5" customHeight="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="16" t="s">
@@ -2470,12 +2469,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A23:R23"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:U26"/>
-    <mergeCell ref="A30:N31"/>
-    <mergeCell ref="A28:U28"/>
     <mergeCell ref="I6:V6"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="I8:M8"/>
@@ -2484,6 +2477,12 @@
     <mergeCell ref="I9:U9"/>
     <mergeCell ref="I5:V5"/>
     <mergeCell ref="I3:V3"/>
+    <mergeCell ref="A23:R23"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:U26"/>
+    <mergeCell ref="A30:N31"/>
+    <mergeCell ref="A28:U28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>